<commit_message>
Add elements.xlsx with 24 rows
</commit_message>
<xml_diff>
--- a/elements.xlsx
+++ b/elements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazar\Desktop\2CM_SmartBuild\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0539BC9-D12E-426F-83CF-5F0876704940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BB0C6B-D638-48B8-8B7C-04A9BEB4648F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{32C24154-C3F7-4F15-A5CF-673C587048DD}"/>
   </bookViews>
@@ -987,11 +987,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C47AF1-1B28-48C5-83B8-C254096ABF78}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>